<commit_message>
changed the style of test cases
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+локал).xlsx
+++ b/Тестовые сценарии (web-камера+локал).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20844D5-56AE-4DCB-999B-44105B3B4075}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E43F783-5C03-4B0D-9B86-324B62B2FDD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Номер сценария </t>
   </si>
@@ -43,19 +43,57 @@
   </si>
   <si>
     <t xml:space="preserve">Проверка инициализации </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIRW S2.0 </t>
   </si>
   <si>
     <t>1. Инициализация «Зритель -Каскад»
 2. Деинициализация «Зритель -Каскад»
-3. Реинициализация «Зритель -Каскад»</t>
-  </si>
-  <si>
-    <t>1. CIRW0001
-2. CIRW0002
-3. CIRW0003</t>
+3. Реинициализация «Зритель -Каскад»
+4. Появление окна с описанием ошибки, когда отключена камера
+5. Появление окна с описанием ошибки, когда нет связи с сервисом</t>
+  </si>
+  <si>
+    <t>Проверить работу «Зритель-Контраст» в АРМ ОПК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.0 </t>
+  </si>
+  <si>
+    <t>CIR-W S2.1</t>
+  </si>
+  <si>
+    <t>1. CIR-W0001
+2. CIR-W0002
+3. CIR-W0003
+4. CIR-W0004
+5. CIR-W0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.2 </t>
+  </si>
+  <si>
+    <t>Проверить форму захвата</t>
+  </si>
+  <si>
+    <t>1. CIR-W0010
+2. CIR-W0011</t>
+  </si>
+  <si>
+    <t>1. Вызов формы захвата с наличием захваченного кадра
+2. Вызов формы захвата без захваченного кадра</t>
+  </si>
+  <si>
+    <t>1. CIR-W0006
+2. CIR-W0007
+3. CIR-W0008
+4. CIR-W0009
+5. CIR-W0012</t>
+  </si>
+  <si>
+    <t>1. Работа «Зритель-контраст» в «АРМ ОПК» 
+2. Захват кадра в главной форме «АРМ ОПК»
+3. Захват кадра на границе окна «Видеокамера»
+4. Отработка таймаута в АРМ ОПК
+5. Вызов формы захвата во время захвата в АРМ ОПК</t>
   </si>
 </sst>
 </file>
@@ -135,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -147,6 +185,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -467,14 +508,14 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
   </cols>
@@ -496,40 +537,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">

</xml_diff>

<commit_message>
changed style on 10 test cases
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+локал).xlsx
+++ b/Тестовые сценарии (web-камера+локал).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E43F783-5C03-4B0D-9B86-324B62B2FDD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054FE0BC-224A-42D7-96E8-07AEAA346321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Номер сценария </t>
   </si>
@@ -75,25 +75,79 @@
   </si>
   <si>
     <t>1. CIR-W0010
-2. CIR-W0011</t>
+2. CIR-W0011
+3. CIR-W0013
+4. CIR-W0014
+5. CIR-W0015</t>
   </si>
   <si>
     <t>1. Вызов формы захвата с наличием захваченного кадра
-2. Вызов формы захвата без захваченного кадра</t>
+2. Вызов формы захвата без захваченного кадра
+3. Нажатие по кнопке «Старт F5» в форме захвата
+4. Нажатие по кнопке «Стоп F6» в форме захвата
+5. Нажатие по кнопке «Закрыть Esc» в форме захвата</t>
   </si>
   <si>
     <t>1. CIR-W0006
 2. CIR-W0007
 3. CIR-W0008
 4. CIR-W0009
-5. CIR-W0012</t>
-  </si>
-  <si>
-    <t>1. Работа «Зритель-контраст» в «АРМ ОПК» 
+5. CIR-W0012
+6. CIR-W0016
+7. CIR-W0017
+8. CIR-W0018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Работа «Зритель-контраст» в «АРМ ОПК» 
 2. Захват кадра в главной форме «АРМ ОПК»
 3. Захват кадра на границе окна «Видеокамера»
 4. Отработка таймаута в АРМ ОПК
-5. Вызов формы захвата во время захвата в АРМ ОПК</t>
+5. Вызов формы захвата во время захвата в АРМ ОПК
+6. Захват с одновременным сканированием документа с ИС
+7. Захват с одновременным сканированием документа без ИС
+8. Отсутствие функции удаления фотографии при нажатии по кнопке «Изменить» </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.3 </t>
+  </si>
+  <si>
+    <t>Проверить отсутствие графических элементов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Отсутствие в списке «Настройка» пункта «Зритель-Каскад»
+2. Отсутствие демо панели в главной форме </t>
+  </si>
+  <si>
+    <t>1. CIR-W0019
+2. CIR-W0020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.4 </t>
+  </si>
+  <si>
+    <t>Проверить работу горячих клавиш в АРМ ОПК</t>
+  </si>
+  <si>
+    <t>1. Отмена выбора кадра сочетанием клавиш Ctrl + F7
+2. Открытие формы захвата сочетанием клавиш Ctrl + F8
+3. Запуск захвата сочетанием клавиш Ctrl + F9</t>
+  </si>
+  <si>
+    <t>1. CIR-W0021
+2. CIR-W0022
+3. CIR-W0023</t>
+  </si>
+  <si>
+    <t>Отключение видоекамеры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Отключение видеокамеры во время захвата </t>
+  </si>
+  <si>
+    <t>1. CIR-W0024</t>
   </si>
 </sst>
 </file>
@@ -507,17 +561,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DDC8C5-BDD2-4180-BFE1-6F2E2D051BB8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -537,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -554,7 +608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -571,7 +625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -588,32 +642,56 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">

</xml_diff>

<commit_message>
changed 7 test cases
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+локал).xlsx
+++ b/Тестовые сценарии (web-камера+локал).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054FE0BC-224A-42D7-96E8-07AEAA346321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDE3D3D-9D98-4BB5-876F-2324C9FD0B3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -74,18 +74,50 @@
     <t>Проверить форму захвата</t>
   </si>
   <si>
-    <t>1. CIR-W0010
-2. CIR-W0011
-3. CIR-W0013
-4. CIR-W0014
-5. CIR-W0015</t>
-  </si>
-  <si>
-    <t>1. Вызов формы захвата с наличием захваченного кадра
-2. Вызов формы захвата без захваченного кадра
-3. Нажатие по кнопке «Старт F5» в форме захвата
-4. Нажатие по кнопке «Стоп F6» в форме захвата
-5. Нажатие по кнопке «Закрыть Esc» в форме захвата</t>
+    <t xml:space="preserve">CIR-W S2.3 </t>
+  </si>
+  <si>
+    <t>Проверить отсутствие графических элементов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Отсутствие в списке «Настройка» пункта «Зритель-Каскад»
+2. Отсутствие демо панели в главной форме </t>
+  </si>
+  <si>
+    <t>1. CIR-W0019
+2. CIR-W0020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.4 </t>
+  </si>
+  <si>
+    <t>Проверить работу горячих клавиш в АРМ ОПК</t>
+  </si>
+  <si>
+    <t>1. Отмена выбора кадра сочетанием клавиш Ctrl + F7
+2. Открытие формы захвата сочетанием клавиш Ctrl + F8
+3. Запуск захвата сочетанием клавиш Ctrl + F9</t>
+  </si>
+  <si>
+    <t>1. CIR-W0021
+2. CIR-W0022
+3. CIR-W0023</t>
+  </si>
+  <si>
+    <t>Отключение видоекамеры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.5 </t>
+  </si>
+  <si>
+    <t>1. CIR-W0024
+2. CIR-W0025
+3. CIR-W0026</t>
+  </si>
+  <si>
+    <t>1. Отключение видеокамеры во время захвата
+2. Кратковременное отключение видеокамеры во время захвата 
+3. Повторный захват после кратковременного отключения</t>
   </si>
   <si>
     <t>1. CIR-W0006
@@ -95,59 +127,43 @@
 5. CIR-W0012
 6. CIR-W0016
 7. CIR-W0017
-8. CIR-W0018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Работа «Зритель-контраст» в «АРМ ОПК» 
+8. CIR-W0018
+9. CIR-W0027
+10. CIR-W0028
+11. CIR-W0029</t>
+  </si>
+  <si>
+    <t>1. Работа «Зритель-контраст» в «АРМ ОПК» 
 2. Захват кадра в главной форме «АРМ ОПК»
 3. Захват кадра на границе окна «Видеокамера»
 4. Отработка таймаута в АРМ ОПК
 5. Вызов формы захвата во время захвата в АРМ ОПК
 6. Захват с одновременным сканированием документа с ИС
 7. Захват с одновременным сканированием документа без ИС
-8. Отсутствие функции удаления фотографии при нажатии по кнопке «Изменить» </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.3 </t>
-  </si>
-  <si>
-    <t>Проверить отсутствие графических элементов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Отсутствие в списке «Настройка» пункта «Зритель-Каскад»
-2. Отсутствие демо панели в главной форме </t>
-  </si>
-  <si>
-    <t>1. CIR-W0019
-2. CIR-W0020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.4 </t>
-  </si>
-  <si>
-    <t>Проверить работу горячих клавиш в АРМ ОПК</t>
-  </si>
-  <si>
-    <t>1. Отмена выбора кадра сочетанием клавиш Ctrl + F7
-2. Открытие формы захвата сочетанием клавиш Ctrl + F8
-3. Запуск захвата сочетанием клавиш Ctrl + F9</t>
-  </si>
-  <si>
-    <t>1. CIR-W0021
-2. CIR-W0022
-3. CIR-W0023</t>
-  </si>
-  <si>
-    <t>Отключение видоекамеры</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Отключение видеокамеры во время захвата </t>
-  </si>
-  <si>
-    <t>1. CIR-W0024</t>
+8. Отсутствие функции удаления фотографии при нажатии по кнопке «Изменить» 
+9. Захват кадра на расстоянии в главной форме АРМ ОПК
+10. Захват кадра на большом расстоянии в главной форме АРМ ОПК
+11. Захват кадра с несколькими лицами, в главной форме АРМ ОПК</t>
+  </si>
+  <si>
+    <t>1. CIR-W0010
+2. CIR-W0011
+3. CIR-W0013
+4. CIR-W0014
+5. CIR-W0015
+6. CIR-W0030
+7. CIR-W0031
+8. CIR-W0032</t>
+  </si>
+  <si>
+    <t>1. Вызов формы захвата с наличием захваченного кадра
+2. Вызов формы захвата без захваченного кадра
+3. Нажатие по кнопке «Старт F5» в форме захвата
+4. Нажатие по кнопке «Стоп F6» в форме захвата
+5. Нажатие по кнопке «Закрыть Esc» в форме захвата
+6. Захват кадра с несколькими лицами в форме захвата
+7. Выбор другого захваченного кадра
+8. Захват кадра на границе области с видеопотоком в форме захвата</t>
   </si>
 </sst>
 </file>
@@ -562,7 +578,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H6" sqref="H5:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +586,7 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,7 +624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="310.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -619,13 +635,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -636,10 +652,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -647,16 +663,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -664,33 +680,33 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
delated old test cases
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+локал).xlsx
+++ b/Тестовые сценарии (web-камера+локал).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDE3D3D-9D98-4BB5-876F-2324C9FD0B3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B65E0A-10B6-442E-99B5-DD8AD856D0D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Номер сценария </t>
   </si>
@@ -153,7 +153,10 @@
 5. CIR-W0015
 6. CIR-W0030
 7. CIR-W0031
-8. CIR-W0032</t>
+8. CIR-W0032
+9. CIR-W0033
+10. CIR-W0034
+11. CIR-W0035</t>
   </si>
   <si>
     <t>1. Вызов формы захвата с наличием захваченного кадра
@@ -163,7 +166,24 @@
 5. Нажатие по кнопке «Закрыть Esc» в форме захвата
 6. Захват кадра с несколькими лицами в форме захвата
 7. Выбор другого захваченного кадра
-8. Захват кадра на границе области с видеопотоком в форме захвата</t>
+8. Захват кадра на границе области с видеопотоком в форме захвата
+9. Считывание документа с ИС, в открытой форме захвата
+10. Считывание документа без ИС, в открытой форме захвата
+11. Повторное считывание документа с открытой формой захвата во время захвата</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.6 </t>
+  </si>
+  <si>
+    <t>Проверка логов</t>
+  </si>
+  <si>
+    <t>1. CIR-W0036
+2. CIR-W0037</t>
+  </si>
+  <si>
+    <t>1. Создание логов «Контраст» при входе в «Система Каскад»
+2. Изображения в папке «captures»</t>
   </si>
 </sst>
 </file>
@@ -577,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DDC8C5-BDD2-4180-BFE1-6F2E2D051BB8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H5:H6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -658,7 +678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -709,14 +729,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
end test scenario for Kascad
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+локал).xlsx
+++ b/Тестовые сценарии (web-камера+локал).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B65E0A-10B6-442E-99B5-DD8AD856D0D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3D8F8-04E3-4C38-A3F5-6D7A7DD7FD9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t xml:space="preserve">Номер сценария </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>ID Сценария</t>
   </si>
@@ -118,6 +115,23 @@
     <t>1. Отключение видеокамеры во время захвата
 2. Кратковременное отключение видеокамеры во время захвата 
 3. Повторный захват после кратковременного отключения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-W S2.6 </t>
+  </si>
+  <si>
+    <t>1. CIR-W0036
+2. CIR-W0037
+3. CIR-W0038
+4. CIR-W0039
+5. CIR-W0040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Создание логов «Контраст» при входе в «Система Каскад»
+2. Изображения в папке «captures»
+3. Начало работы «Контраст» в логах
+4. Конец работы «Контраст» в логах
+5. Инициализация «Контраст-сервиса» </t>
   </si>
   <si>
     <t>1. CIR-W0006
@@ -130,7 +144,8 @@
 8. CIR-W0018
 9. CIR-W0027
 10. CIR-W0028
-11. CIR-W0029</t>
+11. CIR-W0029
+12. CIR-W0041</t>
   </si>
   <si>
     <t>1. Работа «Зритель-контраст» в «АРМ ОПК» 
@@ -143,7 +158,34 @@
 8. Отсутствие функции удаления фотографии при нажатии по кнопке «Изменить» 
 9. Захват кадра на расстоянии в главной форме АРМ ОПК
 10. Захват кадра на большом расстоянии в главной форме АРМ ОПК
-11. Захват кадра с несколькими лицами, в главной форме АРМ ОПК</t>
+11. Захват кадра с несколькими лицами, в главной форме АРМ ОПК
+12. Захват кадра на последних секундах таймаута</t>
+  </si>
+  <si>
+    <t>CIR-W S2.7</t>
+  </si>
+  <si>
+    <t>Проверить логи</t>
+  </si>
+  <si>
+    <t>Проверить верификацию</t>
+  </si>
+  <si>
+    <t>1. Верификация в главной форме АРМ ОПК
+2. Верификация после повторного захвата в  АРМ ОПК
+3. Верификация после повторного считывания документа в АРМ ОПК
+4. Верификация после закрытия формы захвата
+5. Верификация после захвата в форме захвата</t>
+  </si>
+  <si>
+    <t>1. CIR-W0046
+2. CIR-W0047
+3. CIR-W0048
+4. CIR-W0049
+5. CIR-W0050</t>
+  </si>
+  <si>
+    <t>№</t>
   </si>
   <si>
     <t>1. CIR-W0010
@@ -156,7 +198,13 @@
 8. CIR-W0032
 9. CIR-W0033
 10. CIR-W0034
-11. CIR-W0035</t>
+11. CIR-W0035
+12. CIR-W0042
+13. CIR-W0043
+14. CIR-W0044
+15. CIR-W0045
+16. CIR-W0051
+17. CIR-W0052</t>
   </si>
   <si>
     <t>1. Вызов формы захвата с наличием захваченного кадра
@@ -169,21 +217,35 @@
 8. Захват кадра на границе области с видеопотоком в форме захвата
 9. Считывание документа с ИС, в открытой форме захвата
 10. Считывание документа без ИС, в открытой форме захвата
-11. Повторное считывание документа с открытой формой захвата во время захвата</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.6 </t>
-  </si>
-  <si>
-    <t>Проверка логов</t>
-  </si>
-  <si>
-    <t>1. CIR-W0036
-2. CIR-W0037</t>
-  </si>
-  <si>
-    <t>1. Создание логов «Контраст» при входе в «Система Каскад»
-2. Изображения в папке «captures»</t>
+11. Повторное считывание документа с открытой формой захвата во время захвата
+12. Захват кадра на последних секундах таймаута в форме захвата
+13. Захват после таймаута в форме захвата
+14. Закрытие формы захвата во время захвата
+15. Закрытие формы захвата после нажатия на кнопку «Стоп F6» 
+16. Захват кадра на расстоянии в форме захвата
+17. Захват кадра на большом расстоянии в форме захвата</t>
+  </si>
+  <si>
+    <t>CIR-W S2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить работу камеры в разных ориентациях </t>
+  </si>
+  <si>
+    <t>1. CIR-W0053
+2. CIR-W0054
+3. CIR-W0055
+4. CIR-W0056
+5. CIR-W0057
+6. CIR-W0058</t>
+  </si>
+  <si>
+    <t>1. Захват  в главной форме АРМ ОПК с повернутой на 90 градусов камерой по часовой стрелке
+2. Захват в форме захвата с повернутой на 90 градусов камерой по часовой стрелке 
+3. Захват в главной форме АРМ ОПК с повернутой на 180 градусов камерой по часовой стрелке
+4. Захват в форме захвата с повернутой на 180 градусов камерой по часовой стрелке
+5. Захват в главной форме АРМ ОПК с повернутой на 270 градусов камерой по часовой стрелке
+6. Захват в форме захвата с повернутой на 270 градусов камерой по часовой стрелке</t>
   </si>
 </sst>
 </file>
@@ -263,11 +325,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -275,9 +334,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -597,184 +653,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DDC8C5-BDD2-4180-BFE1-6F2E2D051BB8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="310.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>